<commit_message>
Modified Basic_Analysis_Fluo, polarLoc plot script unfinished
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732BFA5D-2435-4E8D-BA29-A658DF43E8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20F3FF-D1C8-4A6B-BC6E-00E985BD322E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6394" yWindow="4431" windowWidth="24686" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5589" yWindow="3077" windowWidth="24685" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="5" r:id="rId1"/>

</xml_diff>

<commit_message>
Added two channel support for basic_analysis
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -8,55 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20F3FF-D1C8-4A6B-BC6E-00E985BD322E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5126FB-8FFF-4600-A9DD-C08C6A0BB176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5589" yWindow="3077" windowWidth="24685" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7106" yWindow="7371" windowWidth="24685" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="5" r:id="rId1"/>
-    <sheet name="FImW Jenal PC" sheetId="41" r:id="rId2"/>
-    <sheet name="FimXW fluo" sheetId="40" r:id="rId3"/>
-    <sheet name="compare FimWs" sheetId="39" r:id="rId4"/>
-    <sheet name="FimW" sheetId="38" r:id="rId5"/>
-    <sheet name="Alternative_Input (HDAEcyaB)" sheetId="37" r:id="rId6"/>
-    <sheet name="Alternative_Input (osc ChpB)" sheetId="36" r:id="rId7"/>
-    <sheet name="Alternative_Input (1297)" sheetId="35" r:id="rId8"/>
-    <sheet name="Alternative_Input (T8V FimXosc)" sheetId="34" r:id="rId9"/>
-    <sheet name="Alternative_Input (PilZ)" sheetId="33" r:id="rId10"/>
-    <sheet name="Alternative_Input (ChpB Ocs A-)" sheetId="32" r:id="rId11"/>
-    <sheet name="Alternative_Input (FimX cAMP O)" sheetId="31" r:id="rId12"/>
-    <sheet name="Alternative_Input (FimX HAE Oc)" sheetId="26" r:id="rId13"/>
-    <sheet name="Alternative_Input (GH-)" sheetId="30" r:id="rId14"/>
-    <sheet name="Alternative_Input (KB-)" sheetId="28" r:id="rId15"/>
-    <sheet name="Alternative_Input (T8Vnew)" sheetId="27" r:id="rId16"/>
-    <sheet name="Alternative_Input (FimX H-)" sheetId="25" r:id="rId17"/>
-    <sheet name="Alternative_Input (FimX HDAE)" sheetId="24" r:id="rId18"/>
-    <sheet name="Alternative_Input (GD58AE)" sheetId="23" r:id="rId19"/>
-    <sheet name="Alternative_Input (FimX K-B-)" sheetId="22" r:id="rId20"/>
-    <sheet name="Alternative_Input (PilK pJN)" sheetId="21" r:id="rId21"/>
-    <sheet name="Alternative_Input (new KB)" sheetId="20" r:id="rId22"/>
-    <sheet name="Alternative_Input (K-B-cB- Rev)" sheetId="11" r:id="rId23"/>
-    <sheet name="Alternative_Input (KB cpdA)" sheetId="17" r:id="rId24"/>
-    <sheet name="Alternative_Input (ChpB mNG)" sheetId="18" r:id="rId25"/>
-    <sheet name="Alternative_Input (Gnew)" sheetId="16" r:id="rId26"/>
-    <sheet name="Alternative_Input (T8V)" sheetId="15" r:id="rId27"/>
-    <sheet name="Alternative_Input (PilH_D52AE)" sheetId="14" r:id="rId28"/>
-    <sheet name="Alternative_Input (Rev J-cA-)" sheetId="13" r:id="rId29"/>
-    <sheet name="Alternative_Input (K-B- Rev)" sheetId="9" r:id="rId30"/>
-    <sheet name="Alternative_Input (T8V Rev)" sheetId="8" r:id="rId31"/>
-    <sheet name="Alternative_Input (OscT8V)" sheetId="7" r:id="rId32"/>
-    <sheet name="Alternative_Input (Osc PilB)" sheetId="10" r:id="rId33"/>
-    <sheet name="Alternative_Input (Reversals)" sheetId="3" r:id="rId34"/>
-    <sheet name="Alternative_Input (FluoFusions)" sheetId="1" r:id="rId35"/>
-    <sheet name="Alternative_Input (Oscillation)" sheetId="6" r:id="rId36"/>
-    <sheet name="Alternative_Input (Pole2Pole)" sheetId="19" r:id="rId37"/>
+    <sheet name="FImW single Jenal Fluo" sheetId="42" r:id="rId2"/>
+    <sheet name="FImW Jenal PC" sheetId="41" r:id="rId3"/>
+    <sheet name="FimXW fluo" sheetId="40" r:id="rId4"/>
+    <sheet name="compare FimWs" sheetId="39" r:id="rId5"/>
+    <sheet name="FimW" sheetId="38" r:id="rId6"/>
+    <sheet name="Alternative_Input (HDAEcyaB)" sheetId="37" r:id="rId7"/>
+    <sheet name="Alternative_Input (osc ChpB)" sheetId="36" r:id="rId8"/>
+    <sheet name="Alternative_Input (1297)" sheetId="35" r:id="rId9"/>
+    <sheet name="Alternative_Input (T8V FimXosc)" sheetId="34" r:id="rId10"/>
+    <sheet name="Alternative_Input (PilZ)" sheetId="33" r:id="rId11"/>
+    <sheet name="Alternative_Input (ChpB Ocs A-)" sheetId="32" r:id="rId12"/>
+    <sheet name="Alternative_Input (FimX cAMP O)" sheetId="31" r:id="rId13"/>
+    <sheet name="Alternative_Input (FimX HAE Oc)" sheetId="26" r:id="rId14"/>
+    <sheet name="Alternative_Input (GH-)" sheetId="30" r:id="rId15"/>
+    <sheet name="Alternative_Input (KB-)" sheetId="28" r:id="rId16"/>
+    <sheet name="Alternative_Input (T8Vnew)" sheetId="27" r:id="rId17"/>
+    <sheet name="Alternative_Input (FimX H-)" sheetId="25" r:id="rId18"/>
+    <sheet name="Alternative_Input (FimX HDAE)" sheetId="24" r:id="rId19"/>
+    <sheet name="Alternative_Input (GD58AE)" sheetId="23" r:id="rId20"/>
+    <sheet name="Alternative_Input (FimX K-B-)" sheetId="22" r:id="rId21"/>
+    <sheet name="Alternative_Input (PilK pJN)" sheetId="21" r:id="rId22"/>
+    <sheet name="Alternative_Input (new KB)" sheetId="20" r:id="rId23"/>
+    <sheet name="Alternative_Input (K-B-cB- Rev)" sheetId="11" r:id="rId24"/>
+    <sheet name="Alternative_Input (KB cpdA)" sheetId="17" r:id="rId25"/>
+    <sheet name="Alternative_Input (ChpB mNG)" sheetId="18" r:id="rId26"/>
+    <sheet name="Alternative_Input (Gnew)" sheetId="16" r:id="rId27"/>
+    <sheet name="Alternative_Input (T8V)" sheetId="15" r:id="rId28"/>
+    <sheet name="Alternative_Input (PilH_D52AE)" sheetId="14" r:id="rId29"/>
+    <sheet name="Alternative_Input (Rev J-cA-)" sheetId="13" r:id="rId30"/>
+    <sheet name="Alternative_Input (K-B- Rev)" sheetId="9" r:id="rId31"/>
+    <sheet name="Alternative_Input (T8V Rev)" sheetId="8" r:id="rId32"/>
+    <sheet name="Alternative_Input (OscT8V)" sheetId="7" r:id="rId33"/>
+    <sheet name="Alternative_Input (Osc PilB)" sheetId="10" r:id="rId34"/>
+    <sheet name="Alternative_Input (Reversals)" sheetId="3" r:id="rId35"/>
+    <sheet name="Alternative_Input (FluoFusions)" sheetId="1" r:id="rId36"/>
+    <sheet name="Alternative_Input (Oscillation)" sheetId="6" r:id="rId37"/>
+    <sheet name="Alternative_Input (Pole2Pole)" sheetId="19" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="95">
   <si>
     <t>5s interval-2h37</t>
   </si>
@@ -338,6 +339,9 @@
   </si>
   <si>
     <t>1638 mNG_FimW pch-</t>
+  </si>
+  <si>
+    <t>1632 mNG_FimW FimX_mScI cpdA</t>
   </si>
 </sst>
 </file>
@@ -1194,15 +1198,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A84C868-F8EF-436A-A77E-F38D40BDB78E}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.4609375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.84375" style="2"/>
@@ -1210,7 +1212,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B1" s="6">
         <v>20220726</v>
@@ -1220,11 +1222,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="8">
-        <v>20220804</v>
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20220728</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -1232,18 +1234,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6">
-        <v>20220726</v>
+        <v>20220729</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
-        <v>80</v>
+      <c r="A4" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B4" s="8">
         <v>20220804</v>
@@ -1253,67 +1255,92 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>93</v>
+      <c r="A5" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B5" s="6">
         <v>20220726</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>93</v>
+      <c r="A6" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B6" s="6">
-        <v>20220728</v>
+        <v>20220729</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7" s="6">
+        <v>20220727</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="6">
+        <v>20220728</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6">
         <v>20220729</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="6">
+        <v>20220727</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="6">
+        <v>20220728</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
+      <c r="A12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6">
+        <v>20220729</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -1323,6 +1350,82 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E4660C-2B7E-4550-A2C2-FC6143C17789}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6">
+        <v>20210810</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6">
+        <v>20210810</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="6">
+        <v>20210810</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="6">
+        <v>20210810</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD30CBFA-FEAD-4F9B-97D2-8D46D9CF912B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1398,7 +1501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397529DF-D713-4447-BBA3-4C154927BDB7}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -1640,7 +1743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151100F7-FFFD-46A0-B10A-96D1CC4471E4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1726,7 +1829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6AC2C3-F7C8-4C03-B191-C5A8CCCCC364}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -1990,7 +2093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18380F9-1431-4DE6-935F-CE91A0490548}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -2171,7 +2274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C35DAA-EA26-4F9F-B405-0AB05C38940A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2275,7 +2378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B26B7D-7EA6-486C-9CAD-6155098EF9EA}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2341,7 +2444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705F7501-BB8E-4FFE-B378-CEC472C3671B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2449,7 +2552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4A07B3-3F53-4259-ABA2-86424D2FCDA9}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2542,7 +2645,136 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC558C1-C908-4D68-87CC-0CA0F615730C}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="6">
+        <v>20220726</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="8">
+        <v>20220804</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="6">
+        <v>20220726</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="8">
+        <v>20220804</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="6">
+        <v>20220726</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="6">
+        <v>20220728</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="6">
+        <v>20220729</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDFEC35-B532-4DE6-9DBB-87A54283D35A}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -2751,62 +2983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D80A3FE-68A1-4C3A-BAC2-168F8E7FE300}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="34.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="6">
-        <v>20220729</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="8">
-        <v>20220804</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="8">
-        <v>20220804</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811F72E5-2D55-4BE7-9EF4-FBBADDB57DE1}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -2941,7 +3118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362DD934-0237-4728-B5F7-54E9408A4A2B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -3025,7 +3202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28511DF-CB7B-4D3F-8294-BDE94D56EA93}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -3139,7 +3316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED93AE3-C6C6-4CF9-989F-42E848236FE0}">
   <dimension ref="A1:C51"/>
   <sheetViews>
@@ -3568,7 +3745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A553FD5-493C-4027-8F83-6AAD22B47920}">
   <dimension ref="A1:F32"/>
   <sheetViews>
@@ -3909,7 +4086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF57C8B-6904-47AA-8A7C-425121F07E92}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -4054,7 +4231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105CD8F9-264D-45C6-88B9-650353853019}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -4276,7 +4453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7D9320-3BD0-4F13-97EB-CCD95C4812EA}">
   <dimension ref="A1:F33"/>
   <sheetViews>
@@ -4535,7 +4712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE5506C-6D25-4A3D-9BBF-307CB4B9DBBB}">
   <dimension ref="A1:M73"/>
   <sheetViews>
@@ -5609,7 +5786,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D80A3FE-68A1-4C3A-BAC2-168F8E7FE300}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="34.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="6">
+        <v>20220729</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="8">
+        <v>20220804</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="8">
+        <v>20220804</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8D2ED9-BB9D-4E75-A276-4347FA42771D}">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -5875,7 +6107,1852 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24CA8E0-F78D-4AF8-A07C-32375F201193}">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.61328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20210120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>20210121</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20210120</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>20210121</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20210120</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>20210121</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39">
+        <v>20210122</v>
+      </c>
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="3">
+        <v>20210120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="2">
+        <v>20210121</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>20210222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3">
+        <v>20210126</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="2">
+        <v>20210126</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="3">
+        <v>20210211</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="3">
+        <v>20210212</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC31EF1D-1F6D-4E42-ACEA-D760942E875D}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>20210114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>20210114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>20210114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>20210114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>20210115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>20210115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>20210115002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>20210122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>20210114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>20210115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>20210114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>20210115</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863DA22-C7EA-4091-BCE1-11E26D2DE89C}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1">
+        <v>20210112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>20210112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>20210112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>20210112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75CF320-837C-4AE5-BE33-E5C2375838A9}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.84375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>20210112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>20210112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0A4CCC-24AB-4E3D-9542-4677F6B08EB8}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>20200916</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>20200918</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>20200924</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>20200916</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>20200918</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>20200924</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>20200916</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>20200918</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>20200924</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>20200916</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>20200918</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>20200924</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>20200916</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>20200918</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>20200924</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>20200916</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>20200922</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>20200929</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>20200916</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>20200918</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>20200924</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>20200916</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>20200918</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>20200924</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>20200916</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>20200922</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>20200929</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <v>20201002</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>20200717</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>20200717</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>20200717</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>20200717</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>20201002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>20201002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>20201002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>20200717</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>20200717</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>20200717</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>20201002</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>20201002</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>20201002</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>20200717</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>20200717</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>20200717</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>20201002</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>20201002</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>20201002</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>20200717</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>20200717</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>20200717</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>20201002</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>20201002</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>20201002</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652C122B-B743-4874-A3B4-AA6D9A3548E9}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20200907</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20200907</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1">
+        <v>20200907</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>20200907</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDB3627-8547-4A88-873C-02CBF702C661}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20200909</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20201008</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20201027</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20201027</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20200908</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>20201027</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>20201027</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>20201029</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>20201029</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22228850-1397-4CB7-B64B-C74620274CBE}">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -6109,1852 +8186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24CA8E0-F78D-4AF8-A07C-32375F201193}">
-  <dimension ref="A1:C60"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.61328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>20210120</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>20210121</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2">
-        <v>20210120</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>20210121</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2">
-        <v>20210120</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>20210121</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39">
-        <v>20210122</v>
-      </c>
-      <c r="C39"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C43" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="3">
-        <v>20210120</v>
-      </c>
-      <c r="C46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="2">
-        <v>20210121</v>
-      </c>
-      <c r="C47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51">
-        <v>20210222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="3">
-        <v>20210126</v>
-      </c>
-      <c r="C52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C55" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C57" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" s="2">
-        <v>20210126</v>
-      </c>
-      <c r="C58" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="3">
-        <v>20210211</v>
-      </c>
-      <c r="C59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" s="3">
-        <v>20210212</v>
-      </c>
-      <c r="C60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC31EF1D-1F6D-4E42-ACEA-D760942E875D}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>20210114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>20210114</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>20210114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>20210114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>20210115</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>20210115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>20210115002</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>20210122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>20210114</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>20210115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>20210114</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>20210115</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863DA22-C7EA-4091-BCE1-11E26D2DE89C}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1">
-        <v>20210112</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>20210112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <v>20210112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>20210112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75CF320-837C-4AE5-BE33-E5C2375838A9}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="22.53515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1">
-        <v>20210112</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>20210112</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0A4CCC-24AB-4E3D-9542-4677F6B08EB8}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>20200916</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>20200918</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>20200924</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>20200916</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>20200918</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>20200924</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>20200916</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>20200918</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>20200924</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>20200916</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>20200918</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>20200924</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>20200916</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>20200918</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>20200924</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>20200916</v>
-      </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>20200922</v>
-      </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>20200929</v>
-      </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>20200916</v>
-      </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>20200918</v>
-      </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>20200924</v>
-      </c>
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>20200916</v>
-      </c>
-      <c r="C22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>20200918</v>
-      </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>20200924</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>20200916</v>
-      </c>
-      <c r="C25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>20200922</v>
-      </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>20200929</v>
-      </c>
-      <c r="C27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1">
-        <v>20201002</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>20200717</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>20200717</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>20200717</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>20200717</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>20201002</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>20201002</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>20201002</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>20200717</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>20200717</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>20200717</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>20201002</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>20201002</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>20201002</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>20200717</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>20200717</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>20200717</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>20201002</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <v>20201002</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>20201002</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21">
-        <v>20200717</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22">
-        <v>20200717</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
-        <v>20200717</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24">
-        <v>20201002</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>20201002</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26">
-        <v>20201002</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652C122B-B743-4874-A3B4-AA6D9A3548E9}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.15234375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20200907</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1">
-        <v>20200907</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1">
-        <v>20200907</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1">
-        <v>20200907</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDB3627-8547-4A88-873C-02CBF702C661}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.15234375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20200909</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>20201008</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1">
-        <v>20201027</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>20201027</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20200908</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20201027</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1">
-        <v>20201027</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>20201029</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>20201029</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE52906-82D3-40B3-B885-A6435708206C}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -8064,7 +8296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209545A1-8AD1-4FA9-8A65-E72255D33C35}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -8196,7 +8428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C583141F-5948-4E26-A05B-357C28402624}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -8306,7 +8538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C7249A-8C4C-40CD-91FC-0F6D34CFF522}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -8384,7 +8616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2D0659-D26C-4493-AB8F-42FA2642647A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -8442,80 +8674,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E4660C-2B7E-4550-A2C2-FC6143C17789}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="29.4609375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.84375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="6">
-        <v>20210810</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="6">
-        <v>20210810</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="6">
-        <v>20210810</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="6">
-        <v>20210810</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added second channel support to cell_prop
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5126FB-8FFF-4600-A9DD-C08C6A0BB176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB848D2-BD6F-4DF8-8FF6-D6D2A72D2B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7106" yWindow="7371" windowWidth="24685" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4551" yWindow="1886" windowWidth="24686" windowHeight="14734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="5" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated graphs with drift corrected data
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4525F4FE-0F09-4BF4-93F5-00A03B1DF726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9811C4-205F-46BA-B12B-531BE5B49343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4671" yWindow="1594" windowWidth="24686" windowHeight="14735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="1654" windowWidth="24686" windowHeight="14735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alternative_Input" sheetId="5" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="94">
   <si>
     <t>5s interval-2h37</t>
   </si>
@@ -1196,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A84C868-F8EF-436A-A77E-F38D40BDB78E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1255,35 +1255,90 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>89</v>
+      <c r="A5" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B5" s="6">
-        <v>20220727</v>
+        <v>20220726</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>89</v>
+      <c r="A6" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B6" s="6">
-        <v>20220728</v>
+        <v>20220729</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="6">
+        <v>20220727</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="6">
+        <v>20220728</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="6">
+        <v>20220729</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B10" s="6">
+        <v>20220727</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="6">
+        <v>20220728</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6">
         <v>20220729</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2562,7 +2617,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A9" sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Moved results folder to shared NAS
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuehn\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EC859C-1350-4FB7-9A8D-CCD8C904721B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA98D69E-CF93-408A-817F-6143FF614246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="76">
   <si>
     <t>5s interval-2h37</t>
   </si>
@@ -1121,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A84C868-F8EF-436A-A77E-F38D40BDB78E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1136,135 +1136,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>68</v>
+      <c r="A1" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="5">
-        <v>20220726</v>
+        <v>20220812</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="5">
-        <v>20220728</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="5">
-        <v>20220729</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="7">
-        <v>20220804</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5">
-        <v>20220726</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="5">
-        <v>20220729</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="5">
-        <v>20220727</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="5">
-        <v>20220728</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="5">
-        <v>20220729</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="5">
-        <v>20220727</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="5">
-        <v>20220728</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="5">
-        <v>20220729</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3693,7 +3572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>

<commit_message>
remove groath curve plotting. update old codes
</commit_message>
<xml_diff>
--- a/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
+++ b/basic_analysis/Matlab_scripts/Data_Input_Basic_Analysis.xlsx
@@ -1,42 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\uppersat-raw\Gani_sv_WS\git\bs_Twitch\basic_analysis\Matlab_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF366D87-BDF5-4A83-86E2-E826C0CEB200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6594B3CE-1FF4-470F-97A6-93A1AC27BEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="3510" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="6" r:id="rId1"/>
-    <sheet name="20231031" sheetId="22" r:id="rId2"/>
-    <sheet name="20230815" sheetId="21" r:id="rId3"/>
-    <sheet name="20230809" sheetId="20" r:id="rId4"/>
-    <sheet name="20230726" sheetId="19" r:id="rId5"/>
-    <sheet name="20230705" sheetId="18" r:id="rId6"/>
-    <sheet name="20230411" sheetId="17" r:id="rId7"/>
-    <sheet name="20230331" sheetId="16" r:id="rId8"/>
-    <sheet name="20230323" sheetId="15" r:id="rId9"/>
-    <sheet name="20230215_fluo" sheetId="14" r:id="rId10"/>
-    <sheet name="20230308_fluo" sheetId="13" r:id="rId11"/>
-    <sheet name="20230308" sheetId="12" r:id="rId12"/>
-    <sheet name="20230221" sheetId="11" r:id="rId13"/>
-    <sheet name="20230215" sheetId="10" r:id="rId14"/>
-    <sheet name="20230131" sheetId="9" r:id="rId15"/>
-    <sheet name="20230126" sheetId="8" r:id="rId16"/>
-    <sheet name="20230124" sheetId="5" r:id="rId17"/>
+    <sheet name="Input" sheetId="25" r:id="rId1"/>
+    <sheet name="Anjali" sheetId="28" r:id="rId2"/>
+    <sheet name="20241018" sheetId="27" r:id="rId3"/>
+    <sheet name="20241011" sheetId="26" r:id="rId4"/>
+    <sheet name="20240813" sheetId="6" r:id="rId5"/>
+    <sheet name="20240712" sheetId="24" r:id="rId6"/>
+    <sheet name="20240326" sheetId="23" r:id="rId7"/>
+    <sheet name="20231031" sheetId="22" r:id="rId8"/>
+    <sheet name="20230815" sheetId="21" r:id="rId9"/>
+    <sheet name="20230809" sheetId="20" r:id="rId10"/>
+    <sheet name="20230726" sheetId="19" r:id="rId11"/>
+    <sheet name="20230705" sheetId="18" r:id="rId12"/>
+    <sheet name="20230411" sheetId="17" r:id="rId13"/>
+    <sheet name="20230331" sheetId="16" r:id="rId14"/>
+    <sheet name="20230323" sheetId="15" r:id="rId15"/>
+    <sheet name="20230215_fluo" sheetId="14" r:id="rId16"/>
+    <sheet name="20230308_fluo" sheetId="13" r:id="rId17"/>
+    <sheet name="20230308" sheetId="12" r:id="rId18"/>
+    <sheet name="20230221" sheetId="11" r:id="rId19"/>
+    <sheet name="20230215" sheetId="10" r:id="rId20"/>
+    <sheet name="20230131" sheetId="9" r:id="rId21"/>
+    <sheet name="20230126" sheetId="8" r:id="rId22"/>
+    <sheet name="20230124" sheetId="5" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
   <si>
     <t>177 fliC-</t>
   </si>
@@ -177,6 +183,84 @@
   </si>
   <si>
     <t>2153 fliC- cyaB- fimV- pCuAlgent_mNG_cyaB CuA20</t>
+  </si>
+  <si>
+    <t>195 pilJ-</t>
+  </si>
+  <si>
+    <t>914 WT</t>
+  </si>
+  <si>
+    <t>2293 3xFLAG PilJ Me1</t>
+  </si>
+  <si>
+    <t>2294 3xFLAG PilJ Me2</t>
+  </si>
+  <si>
+    <t>2295 3xFLAG PilJ Me3</t>
+  </si>
+  <si>
+    <t>1178 fliC- pilA_T8V</t>
+  </si>
+  <si>
+    <t>2453 fliC- pilA_E11L</t>
+  </si>
+  <si>
+    <t>2454 fliC- pilA_Y30T</t>
+  </si>
+  <si>
+    <t>2455 fliC- pilA_R36E</t>
+  </si>
+  <si>
+    <t>2456 fliC- pilA_R36N</t>
+  </si>
+  <si>
+    <t>1047 fliC- pilA-</t>
+  </si>
+  <si>
+    <t>2581 fliC- cyaB- pCuAlgent_mNeonGreen_cyaB_R456L CuA20</t>
+  </si>
+  <si>
+    <t>2583 fliC- cyaB- pilJ- pCuAlgent_mNeonGreen_cyaB_R456L CuA20</t>
+  </si>
+  <si>
+    <t>2584 fliC- cyaB- pilG- pCuAlgent_mNeonGreen_cyaB_R456L CuA20</t>
+  </si>
+  <si>
+    <t>2585 fliC- cyaB- fimL- pCuAlgent_mNeonGreen_cyaB_R456L CuA20</t>
+  </si>
+  <si>
+    <t>2586 fliC- cyaB- chpA- pCuAlgent_mNeonGreen_cyaB_R456L CuA20</t>
+  </si>
+  <si>
+    <t>2634 fliC- pilA_R36A</t>
+  </si>
+  <si>
+    <t>2635 fliC- pilA_E55D</t>
+  </si>
+  <si>
+    <t>2636 fliC- pilA_E55R</t>
+  </si>
+  <si>
+    <t>2637 fliC- pilA_E55A</t>
+  </si>
+  <si>
+    <t>2638 fliC- pilA_A75G</t>
+  </si>
+  <si>
+    <t>2639 A</t>
+  </si>
+  <si>
+    <t>2640 B</t>
+  </si>
+  <si>
+    <t>2650 C</t>
+  </si>
+  <si>
+    <t>2650 D</t>
+  </si>
+  <si>
+    <t>2293 pilJ Me1</t>
   </si>
 </sst>
 </file>
@@ -666,8 +750,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -727,9 +814,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -767,7 +854,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -873,7 +960,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1015,18 +1102,72 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D57CDC3-BE0E-4632-89E2-812A3BBF6243}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06F9512-31AA-4E9A-88B8-03FCD5FCE7AA}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1">
+        <v>20240326</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>20240326</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <v>20240326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD85778-9650-4F20-A4A4-7FC49396979E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1182,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>20231031</v>
+        <v>20230809</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1049,10 +1190,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2">
-        <v>20231031</v>
+        <v>20230809</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1060,21 +1201,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3">
-        <v>20231031</v>
+        <v>20230809</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B4">
-        <v>20231031</v>
+        <v>20230809</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1082,10 +1223,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B5">
-        <v>20231031</v>
+        <v>20230809</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1097,7 +1238,497 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27085A6E-5C7C-4714-AF1E-877224E0D2BA}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>20230726</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>20230726</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>20230726</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>20230726</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>20230726</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75924EC0-7616-46B6-8608-4C6C6A309157}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>20230705</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>20230705</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>20230705</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>20230705</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>20230705</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3987F70B-0420-468F-A227-ACDAD9F04BD3}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>20230411</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>20230411</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>20230411</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>20230411</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>20230411</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>20230411</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B333D9F-8255-4F70-BEEA-78E18AE054EA}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>20230331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>20230331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>20230331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>20230331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>20230331</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>20230331</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>20230331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3F416-AA2B-404C-ADDF-7DCEC724B3C3}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>20230323</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>20230323</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>20230323</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>20230323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>20230323</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>20230323</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>20230323</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>20230323</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>20230323</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>20230323</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>20230323</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>20230323</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC743801-C7EA-49C3-ACC1-FA3EC60086D1}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1184,7 +1815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144790A5-6F0C-47CA-A161-1CBF69679C4A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1337,7 +1968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F891E17-E7F1-4934-8801-EA87373960EC}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1457,7 +2088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC84F82E-74A3-4013-9E5C-C00EDFDFA593}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1522,7 +2153,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A25E4D6-A09D-4DF3-973F-E9C4219D9CAB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1">
+        <v>20241302</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <v>20241302</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>20241302</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>20241302</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7EA1AC-C8C1-4737-8513-C9276683A579}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1587,7 +2283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD35581-7DD1-4666-BD50-5CDB2525AB28}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1652,7 +2348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FAED695-6117-4D23-AA4C-293B5D909356}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1761,7 +2457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A84C868-F8EF-436A-A77E-F38D40BDB78E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1827,7 +2523,497 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4EC762D-ED86-4459-8A28-AE47F069A90A}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>20241018</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>20241018</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>20241018</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>20241018</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>20241018</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>20241018</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7">
+        <v>20241018</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6F170D-9BC2-4952-8F79-119DB5F6B688}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>20241011</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>20241011</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>20241011</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>20241011</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>20241011</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>20241011</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D57CDC3-BE0E-4632-89E2-812A3BBF6243}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>20240813</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>20240813</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>20240813</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>20240813</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>20240813</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>20240813</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>20240813</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6728D691-EBF7-4588-B1EE-9BA35C4CE9A4}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>20240712</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>20240712</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>20240712</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>20240712</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>20240712</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>20240712</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>20240712</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D24CE3-DD25-4A51-935B-027AE60A1BE8}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1">
+        <v>20240326</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>20240326</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>20240326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>20240326</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>20240326</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>20240326</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>20240326</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>20240326</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C380191D-798D-426A-9B95-3CF5D245B999}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1903,7 +3089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265D7EFD-C889-4411-93E4-44F0CE5655F2}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1991,570 +3177,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD85778-9650-4F20-A4A4-7FC49396979E}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1">
-        <v>20230809</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>20230809</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3">
-        <v>20230809</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>20230809</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5">
-        <v>20230809</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27085A6E-5C7C-4714-AF1E-877224E0D2BA}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1">
-        <v>20230726</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <v>20230726</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3">
-        <v>20230726</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>20230726</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5">
-        <v>20230726</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75924EC0-7616-46B6-8608-4C6C6A309157}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1">
-        <v>20230705</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <v>20230705</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>20230705</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>20230705</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>20230705</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3987F70B-0420-468F-A227-ACDAD9F04BD3}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1">
-        <v>20230411</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>20230411</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <v>20230411</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>20230411</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>20230411</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>20230411</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B333D9F-8255-4F70-BEEA-78E18AE054EA}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1">
-        <v>20230331</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2">
-        <v>20230331</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>20230331</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>20230331</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>20230331</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>20230331</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>20230331</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3F416-AA2B-404C-ADDF-7DCEC724B3C3}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1">
-        <v>20230323</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>20230323</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>20230323</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <v>20230323</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5">
-        <v>20230323</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6">
-        <v>20230323</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>20230323</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8">
-        <v>20230323</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>20230323</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>20230323</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>20230323</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>20230323</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>